<commit_message>
Added velpatasvir and pibrentasvir in vitro / subtype 3a findings from Smith et al 2018.
</commit_message>
<xml_diff>
--- a/tabular/contributed/180629 GLE PIB TABLE.xlsx
+++ b/tabular/contributed/180629 GLE PIB TABLE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12980" yWindow="2440" windowWidth="50120" windowHeight="28340" activeTab="1"/>
+    <workbookView xWindow="6440" yWindow="460" windowWidth="50120" windowHeight="28340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GLE" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="136">
   <si>
     <t>in vivo</t>
   </si>
@@ -428,6 +428,15 @@
   </si>
   <si>
     <t>EASL_2017_FRI_205</t>
+  </si>
+  <si>
+    <t>30K+31M</t>
+  </si>
+  <si>
+    <t>30K+31M+93H</t>
+  </si>
+  <si>
+    <t>&gt;20</t>
   </si>
 </sst>
 </file>
@@ -540,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -715,6 +724,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3897,11 +3912,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7028,6 +7043,93 @@
         <v>132</v>
       </c>
       <c r="O69" s="61"/>
+    </row>
+    <row r="70" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H70" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="I70" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="N70" s="66">
+        <v>29425396</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G71" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="I71" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="N71" s="66">
+        <v>29425396</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="D72" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G72" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H72" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="I72" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="N72" s="66">
+        <v>29425396</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:O71">

</xml_diff>